<commit_message>
Updates to add trace file.
</commit_message>
<xml_diff>
--- a/study_guides/midterm_1_review/tophat_vliw_scheduling_answer.xlsx
+++ b/study_guides/midterm_1_review/tophat_vliw_scheduling_answer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrabb\Desktop\Wonsun Ahn\cs1541\CS1541_Fall2020\study_guides\midterm_1_review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19CF030-18BB-4E56-A45E-2377459C405E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87E67D6-4CBE-48B5-8A97-43CB090FB835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13905" yWindow="1155" windowWidth="19650" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8655" yWindow="405" windowWidth="19650" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>Assume split instruction and data memory, full data forwarding, and perfect branch prediction (with both BHT and BTB).</t>
   </si>
   <si>
-    <t>* Can be simulated using the 2-wide-opt.conf and midterm_1_review.tr trace.  The result is going be for an in-order superscalar but the only difference for a VLIW is that instead of the hazard detection unit inserting bubbles, the compiler schedules instructions so that there are no hazards.</t>
-  </si>
-  <si>
     <t>lw t0, 0(s1)</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>addi t2, t1, 4</t>
+  </si>
+  <si>
+    <t>* Can be simulated using the 2-wide-opt.conf and tophat_vliw_scheduling.tr trace.  The result is going be for an in-order superscalar but the only difference for a VLIW is that instead of the hazard detection unit inserting bubbles, the compiler schedules instructions so that there are no hazards.</t>
   </si>
 </sst>
 </file>
@@ -152,6 +152,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -159,9 +162,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,7 +446,7 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,64 +456,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
@@ -625,7 +625,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -705,7 +705,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -744,7 +744,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -810,34 +810,34 @@
       <c r="Z9" s="5"/>
     </row>
     <row r="10" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
-      <c r="Z10" s="7"/>
+      <c r="A10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
@@ -868,209 +868,212 @@
       <c r="Z11" s="5"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="9"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8" t="s">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>1</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>2</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6" t="s">
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>3</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6" t="s">
+      <c r="B17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>4</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6" t="s">
+      <c r="B18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>5</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6" t="s">
+      <c r="B19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>6</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>7</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>8</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>9</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>10</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:Z1"/>
-    <mergeCell ref="A2:Z2"/>
-    <mergeCell ref="A12:Z12"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="B21:E21"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="A10:Z10"/>
@@ -1084,14 +1087,11 @@
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="F20:I20"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="A1:Z1"/>
+    <mergeCell ref="A2:Z2"/>
+    <mergeCell ref="A12:Z12"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>